<commit_message>
:hammer: change template file part
</commit_message>
<xml_diff>
--- a/public/templates/Template_Upload_Part.xlsx
+++ b/public/templates/Template_Upload_Part.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Project\metronic\metronic-react\public\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36DE7EE2-AD55-45F5-8BDD-968A7E1D5708}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{796DA9B6-E9AD-47A2-BE93-EC6879DDD68D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2550" yWindow="2550" windowWidth="21600" windowHeight="11385" xr2:uid="{ABF8BF26-C2A3-4507-A836-51312AD95510}"/>
+    <workbookView xWindow="7215" yWindow="4365" windowWidth="21600" windowHeight="11385" xr2:uid="{ABF8BF26-C2A3-4507-A836-51312AD95510}"/>
   </bookViews>
   <sheets>
-    <sheet name="case_category" sheetId="1" r:id="rId1"/>
+    <sheet name="part" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -426,7 +426,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>